<commit_message>
Updated budget and PCB
</commit_message>
<xml_diff>
--- a/Électronique/Admin/Electronic budget planing.xlsx
+++ b/Électronique/Admin/Electronic budget planing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulavaldti-my.sharepoint.com/personal/matot9_ulaval_ca/Documents/Github/design3/Électronique/Admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1330" documentId="8_{F4AF0EF8-8E10-4CF9-8076-0BC56F572DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F274C83-B03C-46CB-8A45-DEE599881E12}"/>
+  <xr:revisionPtr revIDLastSave="1543" documentId="8_{F4AF0EF8-8E10-4CF9-8076-0BC56F572DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDC28E99-19EC-42D1-B3C0-E44723BFB3F3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EB5A697F-0613-4937-9779-A2AEDA335630}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{EB5A697F-0613-4937-9779-A2AEDA335630}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition channel" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="140">
   <si>
     <t>Qty</t>
   </si>
@@ -153,12 +153,6 @@
     <t>Series Voltage Reference IC Fixed 3.3V V ±0.1%</t>
   </si>
   <si>
-    <t>MCP1501-18E/SN</t>
-  </si>
-  <si>
-    <t>MCP1501-18E/SN-ND</t>
-  </si>
-  <si>
     <t>Power Barrel Connector Jack 2.10mm</t>
   </si>
   <si>
@@ -216,12 +210,6 @@
     <t>Socket Strips, .050" Pitch</t>
   </si>
   <si>
-    <t>SFSD-20-28-G-10.00-DR-NDS</t>
-  </si>
-  <si>
-    <t>Double Row Discrete Wire Cable Assembly, Socket</t>
-  </si>
-  <si>
     <t>Power Supply Wall Adapter</t>
   </si>
   <si>
@@ -369,24 +357,6 @@
     <t>SAM13327CT-ND</t>
   </si>
   <si>
-    <t>20 pins rect conect Housings Insulator 0.05'' pitch</t>
-  </si>
-  <si>
-    <t>ISDF-10-D</t>
-  </si>
-  <si>
-    <t>SAM9647-ND</t>
-  </si>
-  <si>
-    <t>TFM-110-01-L-D-A</t>
-  </si>
-  <si>
-    <t>612-TFM-110-01-L-D-A-ND</t>
-  </si>
-  <si>
-    <t>Connector Header 20 position 0.050" pitch</t>
-  </si>
-  <si>
     <t>CONN HSG 20POS 1.27MM</t>
   </si>
   <si>
@@ -399,13 +369,94 @@
     <t>SAM12821-ND</t>
   </si>
   <si>
-    <t>IRF9388TRPBFCT-ND</t>
-  </si>
-  <si>
     <t>IRLML9303TRPBF</t>
   </si>
   <si>
     <t>IRLML9303TRPBFCT-ND</t>
+  </si>
+  <si>
+    <t>Green 530nm LED Indication</t>
+  </si>
+  <si>
+    <t>Würth Elektronik</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>MCP1501T-18E/CHY</t>
+  </si>
+  <si>
+    <t>MCP1501T-18E/CHYCT-ND</t>
+  </si>
+  <si>
+    <t>Red 624nm LED Indication</t>
+  </si>
+  <si>
+    <t>CreeLED, Inc.</t>
+  </si>
+  <si>
+    <t>C503B-RAN-CZ0C0AA2</t>
+  </si>
+  <si>
+    <t>C503B-RAN-CZ0C0AA2CT-ND</t>
+  </si>
+  <si>
+    <t>151053GS03000</t>
+  </si>
+  <si>
+    <t>732-5020-ND</t>
+  </si>
+  <si>
+    <t>4.7 µH Shielded Multilayer Inductor</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
+    <t>ILSB1206ER4R7K</t>
+  </si>
+  <si>
+    <t>541-4372-1-ND</t>
+  </si>
+  <si>
+    <t>2.2 µF ±10% 6.3V Ceramic Capacitor X7R</t>
+  </si>
+  <si>
+    <t>CC0603KRX7R5BB225</t>
+  </si>
+  <si>
+    <t>311-1795-1-ND</t>
+  </si>
+  <si>
+    <t>0.22 µF ±10% 25V Ceramic Capacitor X7R</t>
+  </si>
+  <si>
+    <t>Murata Electronics</t>
+  </si>
+  <si>
+    <t>GRM188R71E224KA88D</t>
+  </si>
+  <si>
+    <t>490-3290-1-ND</t>
+  </si>
+  <si>
+    <t>22.1 kOhms ±1% 0.1W, 1/10W Chip Resistor</t>
+  </si>
+  <si>
+    <t>541-5271-1-ND</t>
+  </si>
+  <si>
+    <t>CRCW060322K1FKEAC</t>
+  </si>
+  <si>
+    <t>CRCW060388K7FKEB</t>
+  </si>
+  <si>
+    <t>88.7 kOhms ±1% 0.1W, 1/10W Chip Resistor</t>
+  </si>
+  <si>
+    <t>541-CRCW060388K7FKEBCT-ND</t>
   </si>
 </sst>
 </file>
@@ -725,7 +776,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -856,9 +907,6 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -943,35 +991,35 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -979,24 +1027,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1050,24 +1092,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1427,51 +1451,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A14AF596-72B6-4068-B240-BE4D8ECB5EC6}">
-  <dimension ref="B1:O70"/>
+  <dimension ref="B1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34:J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="34.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="37.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="21.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.41796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50.15625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.26171875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="37.26171875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.68359375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.41796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.15625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="21.15625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="17.68359375" style="1" customWidth="1"/>
     <col min="13" max="13" width="30" style="1" customWidth="1"/>
     <col min="14" max="14" width="22" style="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.42578125" style="1"/>
+    <col min="15" max="15" width="21.578125" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.41796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:15" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="100" t="s">
+    <row r="1" spans="2:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="2" spans="2:15" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B2" s="97" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="101"/>
-      <c r="I2" s="101"/>
-      <c r="J2" s="102"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="99"/>
       <c r="L2" s="20"/>
       <c r="M2" s="20"/>
       <c r="N2" s="20"/>
       <c r="O2" s="20"/>
     </row>
-    <row r="3" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="19" t="s">
         <v>3</v>
       </c>
@@ -1497,12 +1521,12 @@
       <c r="J3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="51"/>
+      <c r="L3" s="50"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1529,18 +1553,18 @@
         <f>I4*H4</f>
         <v>2.72</v>
       </c>
-      <c r="L4" s="105" t="s">
+      <c r="L4" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="106"/>
-      <c r="N4" s="49" t="s">
+      <c r="M4" s="103"/>
+      <c r="N4" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="O4" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="O4" s="60" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
@@ -1567,16 +1591,16 @@
         <f>I5*H5</f>
         <v>1.56</v>
       </c>
-      <c r="L5" s="107" t="s">
-        <v>76</v>
-      </c>
-      <c r="M5" s="108"/>
-      <c r="N5" s="63">
+      <c r="L5" s="104" t="s">
+        <v>72</v>
+      </c>
+      <c r="M5" s="105"/>
+      <c r="N5" s="62">
         <v>300</v>
       </c>
-      <c r="O5" s="64"/>
-    </row>
-    <row r="6" spans="2:15" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O5" s="63"/>
+    </row>
+    <row r="6" spans="2:15" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B6" s="10" t="s">
         <v>16</v>
       </c>
@@ -1596,31 +1620,31 @@
       <c r="H6" s="11">
         <v>1</v>
       </c>
-      <c r="I6" s="45">
+      <c r="I6" s="44">
         <v>2.68</v>
       </c>
       <c r="J6" s="18">
         <f>I6*H6</f>
         <v>2.68</v>
       </c>
-      <c r="L6" s="89" t="s">
-        <v>72</v>
-      </c>
-      <c r="M6" s="90"/>
-      <c r="N6" s="46">
+      <c r="L6" s="84" t="s">
+        <v>68</v>
+      </c>
+      <c r="M6" s="85"/>
+      <c r="N6" s="45">
         <v>0</v>
       </c>
-      <c r="O6" s="65"/>
-    </row>
-    <row r="7" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="98" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="99"/>
-      <c r="D7" s="99"/>
-      <c r="E7" s="99"/>
-      <c r="F7" s="99"/>
-      <c r="G7" s="99"/>
+      <c r="O6" s="64"/>
+    </row>
+    <row r="7" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="95" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="96"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="96"/>
       <c r="H7" s="35">
         <v>8</v>
       </c>
@@ -1628,31 +1652,31 @@
         <f>SUM(J4:J5)</f>
         <v>4.28</v>
       </c>
-      <c r="J7" s="52">
+      <c r="J7" s="51">
         <f>H7*I7</f>
         <v>34.24</v>
       </c>
-      <c r="L7" s="89" t="s">
-        <v>74</v>
-      </c>
-      <c r="M7" s="90"/>
-      <c r="N7" s="66">
+      <c r="L7" s="84" t="s">
+        <v>70</v>
+      </c>
+      <c r="M7" s="85"/>
+      <c r="N7" s="65">
         <v>0</v>
       </c>
-      <c r="O7" s="67">
-        <f>J49</f>
+      <c r="O7" s="66">
+        <f>J51</f>
         <v>99.8</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="83" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="84"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="84"/>
+    <row r="8" spans="2:15" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B8" s="82" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="83"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="83"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="83"/>
       <c r="H8" s="11">
         <v>8</v>
       </c>
@@ -1664,19 +1688,19 @@
         <f>H8*I8</f>
         <v>55.680000000000007</v>
       </c>
-      <c r="L8" s="89" t="s">
-        <v>75</v>
-      </c>
-      <c r="M8" s="90"/>
-      <c r="N8" s="66">
+      <c r="L8" s="84" t="s">
+        <v>71</v>
+      </c>
+      <c r="M8" s="85"/>
+      <c r="N8" s="65">
         <v>0</v>
       </c>
-      <c r="O8" s="67">
+      <c r="O8" s="66">
         <f>J14</f>
-        <v>117.89399999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>123.855</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1686,16 +1710,16 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="L9" s="89" t="s">
-        <v>82</v>
-      </c>
-      <c r="M9" s="90"/>
-      <c r="N9" s="68">
+      <c r="L9" s="84" t="s">
+        <v>78</v>
+      </c>
+      <c r="M9" s="85"/>
+      <c r="N9" s="67">
         <v>154</v>
       </c>
-      <c r="O9" s="65"/>
-    </row>
-    <row r="10" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O9" s="64"/>
+    </row>
+    <row r="10" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1705,12 +1729,17 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="L10" s="81"/>
-      <c r="M10" s="82"/>
-      <c r="N10" s="68"/>
-      <c r="O10" s="65"/>
-    </row>
-    <row r="11" spans="2:15" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M10" s="16"/>
+      <c r="N10" s="67">
+        <f>J8</f>
+        <v>55.680000000000007</v>
+      </c>
+      <c r="O10" s="64"/>
+    </row>
+    <row r="11" spans="2:15" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -1719,40 +1748,40 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="L11" s="89" t="s">
-        <v>17</v>
-      </c>
-      <c r="M11" s="90"/>
-      <c r="N11" s="68">
-        <f>J8</f>
-        <v>55.680000000000007</v>
-      </c>
-      <c r="O11" s="65"/>
-    </row>
-    <row r="12" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="100" t="s">
+      <c r="L11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="M11" s="16"/>
+      <c r="N11" s="67">
+        <f>J39</f>
+        <v>22.080000000000002</v>
+      </c>
+      <c r="O11" s="64"/>
+    </row>
+    <row r="12" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B12" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="101"/>
-      <c r="D12" s="101"/>
-      <c r="E12" s="101"/>
-      <c r="F12" s="101"/>
-      <c r="G12" s="101"/>
-      <c r="H12" s="101"/>
-      <c r="I12" s="101"/>
-      <c r="J12" s="102"/>
+      <c r="C12" s="98"/>
+      <c r="D12" s="98"/>
+      <c r="E12" s="98"/>
+      <c r="F12" s="98"/>
+      <c r="G12" s="98"/>
+      <c r="H12" s="98"/>
+      <c r="I12" s="98"/>
+      <c r="J12" s="99"/>
       <c r="K12" s="20"/>
-      <c r="L12" s="89" t="s">
-        <v>78</v>
-      </c>
-      <c r="M12" s="90"/>
-      <c r="N12" s="68">
-        <f>J37</f>
-        <v>19.89</v>
-      </c>
-      <c r="O12" s="65"/>
-    </row>
-    <row r="13" spans="2:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L12" s="80" t="s">
+        <v>76</v>
+      </c>
+      <c r="M12" s="81"/>
+      <c r="N12" s="67">
+        <f>J23</f>
+        <v>98.28</v>
+      </c>
+      <c r="O12" s="64"/>
+    </row>
+    <row r="13" spans="2:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="19" t="s">
         <v>3</v>
       </c>
@@ -1779,55 +1808,56 @@
         <v>2</v>
       </c>
       <c r="K13" s="3"/>
-      <c r="L13" s="109" t="s">
-        <v>80</v>
-      </c>
-      <c r="M13" s="110"/>
-      <c r="N13" s="68">
-        <f>J26</f>
-        <v>98.28</v>
-      </c>
-      <c r="O13" s="65"/>
-    </row>
-    <row r="14" spans="2:15" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L13" s="80" t="s">
+        <v>75</v>
+      </c>
+      <c r="M13" s="81"/>
+      <c r="N13" s="67">
+        <f>J63</f>
+        <v>15.979999999999999</v>
+      </c>
+      <c r="O13" s="64"/>
+    </row>
+    <row r="14" spans="2:15" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B14" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>27</v>
       </c>
       <c r="G14" s="11"/>
       <c r="H14" s="11">
-        <v>70</v>
-      </c>
-      <c r="I14" s="47">
-        <v>1.6841999999999999</v>
+        <v>75</v>
+      </c>
+      <c r="I14" s="46">
+        <f>IF(H14&lt;5,2.82,IF(H14&lt;10,2.724,IF(H14&lt;25,2.213,IF(H14&lt;50,1.9072,IF(H14&lt;100,1.6514,IF(H14&lt;500,1.4983,0))))))</f>
+        <v>1.6514</v>
       </c>
       <c r="J14" s="18">
         <f>I14*H14</f>
-        <v>117.89399999999999</v>
+        <v>123.855</v>
       </c>
       <c r="K14" s="2"/>
-      <c r="L14" s="109" t="s">
-        <v>79</v>
-      </c>
-      <c r="M14" s="110"/>
+      <c r="L14" s="82" t="s">
+        <v>54</v>
+      </c>
+      <c r="M14" s="83"/>
       <c r="N14" s="68">
-        <f>J61</f>
-        <v>14.719999999999999</v>
-      </c>
-      <c r="O14" s="65"/>
-    </row>
-    <row r="15" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f>G70</f>
+        <v>41.8095</v>
+      </c>
+      <c r="O14" s="38"/>
+    </row>
+    <row r="15" spans="2:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="5"/>
@@ -1835,20 +1865,20 @@
       <c r="F15" s="5"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="46"/>
+      <c r="I15" s="45"/>
       <c r="J15" s="9"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="83" t="s">
-        <v>56</v>
-      </c>
-      <c r="M15" s="84"/>
-      <c r="N15" s="69">
-        <f>G68</f>
-        <v>70.119</v>
-      </c>
-      <c r="O15" s="38"/>
-    </row>
-    <row r="16" spans="2:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L15" s="86" t="s">
+        <v>79</v>
+      </c>
+      <c r="M15" s="87"/>
+      <c r="N15" s="78">
+        <f>SUM(N5:N6)-SUM(N9:N14)</f>
+        <v>-87.829500000000053</v>
+      </c>
+      <c r="O15" s="79"/>
+    </row>
+    <row r="16" spans="2:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="5"/>
@@ -1856,20 +1886,20 @@
       <c r="F16" s="5"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="46"/>
+      <c r="I16" s="45"/>
       <c r="J16" s="9"/>
       <c r="K16" s="2"/>
-      <c r="L16" s="85" t="s">
-        <v>83</v>
-      </c>
-      <c r="M16" s="86"/>
-      <c r="N16" s="87">
-        <f>SUM(N5:N6)-SUM(N9:N15)</f>
-        <v>-112.68900000000008</v>
-      </c>
-      <c r="O16" s="88"/>
-    </row>
-    <row r="17" spans="2:15" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L16" s="84" t="s">
+        <v>80</v>
+      </c>
+      <c r="M16" s="85"/>
+      <c r="N16" s="72">
+        <f>0.15*-N15</f>
+        <v>13.174425000000008</v>
+      </c>
+      <c r="O16" s="77"/>
+    </row>
+    <row r="17" spans="2:15" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
       <c r="D17" s="2"/>
@@ -1878,39 +1908,38 @@
       <c r="G17" s="2"/>
       <c r="H17" s="6"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="89" t="s">
-        <v>84</v>
-      </c>
-      <c r="M17" s="90"/>
-      <c r="N17" s="77">
-        <f>0.15*-N16</f>
-        <v>16.90335000000001</v>
-      </c>
-      <c r="O17" s="78"/>
-    </row>
-    <row r="18" spans="2:15" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="100" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="101"/>
-      <c r="D18" s="101"/>
-      <c r="E18" s="101"/>
-      <c r="F18" s="101"/>
-      <c r="G18" s="101"/>
-      <c r="H18" s="101"/>
-      <c r="I18" s="101"/>
-      <c r="J18" s="102"/>
+      <c r="L17" s="84" t="s">
+        <v>81</v>
+      </c>
+      <c r="M17" s="85"/>
+      <c r="N17" s="8">
+        <v>0</v>
+      </c>
+      <c r="O17" s="54"/>
+    </row>
+    <row r="18" spans="2:15" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B18" s="97" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="98"/>
+      <c r="D18" s="98"/>
+      <c r="E18" s="98"/>
+      <c r="F18" s="98"/>
+      <c r="G18" s="98"/>
+      <c r="H18" s="98"/>
+      <c r="I18" s="98"/>
+      <c r="J18" s="99"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="89" t="s">
+      <c r="L18" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="M18" s="90"/>
-      <c r="N18" s="79">
-        <v>0</v>
-      </c>
-      <c r="O18" s="80"/>
-    </row>
-    <row r="19" spans="2:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M18" s="16"/>
+      <c r="N18" s="72">
+        <v>10</v>
+      </c>
+      <c r="O18" s="77"/>
+    </row>
+    <row r="19" spans="2:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B19" s="19" t="s">
         <v>3</v>
       </c>
@@ -1936,30 +1965,31 @@
       <c r="J19" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="L19" s="89" t="s">
-        <v>89</v>
-      </c>
-      <c r="M19" s="90"/>
-      <c r="N19" s="77">
-        <v>10</v>
-      </c>
-      <c r="O19" s="78"/>
-    </row>
-    <row r="20" spans="2:15" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L19" s="93" t="s">
+        <v>28</v>
+      </c>
+      <c r="M19" s="94"/>
+      <c r="N19" s="100">
+        <f>N15-N16-N18</f>
+        <v>-111.00392500000007</v>
+      </c>
+      <c r="O19" s="101"/>
+    </row>
+    <row r="20" spans="2:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="36" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2">
@@ -1969,615 +1999,601 @@
         <v>6.87</v>
       </c>
       <c r="J20" s="7">
-        <f>I20*H20</f>
+        <f t="shared" ref="J20:J22" si="0">I20*H20</f>
         <v>54.96</v>
       </c>
-      <c r="L20" s="96" t="s">
-        <v>28</v>
-      </c>
-      <c r="M20" s="97"/>
-      <c r="N20" s="103">
-        <f>N16-N17-N19</f>
-        <v>-139.5923500000001</v>
-      </c>
-      <c r="O20" s="104"/>
-    </row>
-    <row r="21" spans="2:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="2:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="36" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2">
-        <v>0</v>
-      </c>
-      <c r="I21" s="6">
-        <v>1.5189999999999999</v>
+        <v>100</v>
+      </c>
+      <c r="I21" s="75">
+        <f>IF(H21&lt;10,0.29,IF(H21&lt;25,0.246,IF(H21&lt;50,0.2184,IF(H21&lt;100,0.2038,IF(H21&lt;250,0.1892,0)))))</f>
+        <v>0.18920000000000001</v>
       </c>
       <c r="J21" s="7">
-        <f>I21*H21</f>
-        <v>0</v>
-      </c>
-      <c r="L21" s="111"/>
-      <c r="M21" s="111"/>
-      <c r="N21" s="74"/>
-      <c r="O21" s="74"/>
-    </row>
-    <row r="22" spans="2:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>18.920000000000002</v>
+      </c>
+      <c r="L21" s="74"/>
+      <c r="M21" s="74"/>
+      <c r="N21" s="72"/>
+      <c r="O21" s="72"/>
+    </row>
+    <row r="22" spans="2:15" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B22" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>109</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2">
-        <v>100</v>
-      </c>
-      <c r="I22" s="112">
-        <v>0.18920000000000001</v>
+        <v>8</v>
+      </c>
+      <c r="I22" s="6">
+        <v>3.05</v>
       </c>
       <c r="J22" s="7">
-        <f>I22*H22</f>
-        <v>18.920000000000002</v>
-      </c>
-      <c r="L22" s="111"/>
-      <c r="M22" s="111"/>
-      <c r="N22" s="74"/>
-      <c r="O22" s="74"/>
-    </row>
-    <row r="23" spans="2:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2">
-        <v>8</v>
-      </c>
-      <c r="I23" s="6">
-        <v>3.05</v>
-      </c>
-      <c r="J23" s="7">
-        <f>I23*H23</f>
+        <f t="shared" si="0"/>
         <v>24.4</v>
       </c>
-      <c r="L23" s="111"/>
-      <c r="M23" s="111"/>
-      <c r="N23" s="74"/>
-      <c r="O23" s="74"/>
-    </row>
-    <row r="24" spans="2:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="36" t="s">
-        <v>115</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="L22" s="74"/>
+      <c r="M22" s="74"/>
+      <c r="N22" s="72"/>
+      <c r="O22" s="72"/>
+    </row>
+    <row r="23" spans="2:15" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B23" s="88" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="89"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="89"/>
+      <c r="G23" s="89"/>
+      <c r="H23" s="89"/>
+      <c r="I23" s="89"/>
+      <c r="J23" s="49">
+        <f>SUM(J20:J22)</f>
+        <v>98.28</v>
+      </c>
+      <c r="L23" s="61"/>
+      <c r="M23" s="61"/>
+      <c r="N23" s="60"/>
+    </row>
+    <row r="24" spans="2:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="2">
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="L24" s="61"/>
+      <c r="M24" s="61"/>
+      <c r="N24" s="60"/>
+    </row>
+    <row r="25" spans="2:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="N25" s="60"/>
+    </row>
+    <row r="26" spans="2:15" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="2:15" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B27" s="97" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="98"/>
+      <c r="D27" s="98"/>
+      <c r="E27" s="98"/>
+      <c r="F27" s="98"/>
+      <c r="G27" s="98"/>
+      <c r="H27" s="98"/>
+      <c r="I27" s="98"/>
+      <c r="J27" s="99"/>
+    </row>
+    <row r="28" spans="2:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B28" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="I24" s="6">
-        <v>8.85</v>
-      </c>
-      <c r="J24" s="7">
-        <f>I24*H24</f>
-        <v>0</v>
-      </c>
-      <c r="L24" s="111"/>
-      <c r="M24" s="111"/>
-      <c r="N24" s="74"/>
-      <c r="O24" s="74"/>
-    </row>
-    <row r="25" spans="2:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2">
-        <v>0</v>
-      </c>
-      <c r="I25" s="8">
-        <v>16</v>
-      </c>
-      <c r="J25" s="7">
-        <f>I25*H25</f>
-        <v>0</v>
-      </c>
-      <c r="L25" s="113"/>
-      <c r="M25" s="113"/>
-      <c r="N25" s="114"/>
-      <c r="O25" s="114"/>
-    </row>
-    <row r="26" spans="2:15" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="91" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="92"/>
-      <c r="D26" s="92"/>
-      <c r="E26" s="92"/>
-      <c r="F26" s="92"/>
-      <c r="G26" s="92"/>
-      <c r="H26" s="92"/>
-      <c r="I26" s="92"/>
-      <c r="J26" s="50">
-        <f>SUM(J20:J25)</f>
-        <v>98.28</v>
-      </c>
-      <c r="L26" s="62"/>
-      <c r="M26" s="62"/>
-      <c r="N26" s="61"/>
-    </row>
-    <row r="27" spans="2:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="L27" s="62"/>
-      <c r="M27" s="62"/>
-      <c r="N27" s="61"/>
-    </row>
-    <row r="28" spans="2:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="N28" s="61"/>
-    </row>
-    <row r="29" spans="2:15" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="I28" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J28" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B29" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="2:15" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="100" t="s">
-        <v>81</v>
-      </c>
-      <c r="C30" s="101"/>
-      <c r="D30" s="101"/>
-      <c r="E30" s="101"/>
-      <c r="F30" s="101"/>
-      <c r="G30" s="101"/>
-      <c r="H30" s="101"/>
-      <c r="I30" s="101"/>
-      <c r="J30" s="102"/>
-    </row>
-    <row r="31" spans="2:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="19" t="s">
+      <c r="H29" s="2">
+        <v>10</v>
+      </c>
+      <c r="I29" s="42">
+        <f>IF(H29&lt;10,1.52,IF(H29&lt;25,1.332,0))</f>
+        <v>1.3320000000000001</v>
+      </c>
+      <c r="J29" s="7">
+        <f>I29*H29</f>
+        <v>13.32</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B30" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2">
+        <v>1</v>
+      </c>
+      <c r="I30" s="8">
+        <v>0.73</v>
+      </c>
+      <c r="J30" s="7">
+        <f t="shared" ref="J30:J36" si="1">I30*H30</f>
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2">
         <v>3</v>
       </c>
-      <c r="C31" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="I31" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="J31" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="2:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="36" t="s">
-        <v>24</v>
+      <c r="I31" s="8">
+        <f>IF(H31&lt;10,0.33,IF(H31&lt;25,0.295,0))</f>
+        <v>0.33</v>
+      </c>
+      <c r="J31" s="7">
+        <f t="shared" si="1"/>
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32" s="73" t="s">
+        <v>127</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>32</v>
+        <v>128</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>31</v>
+        <v>129</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>7</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2">
-        <v>10</v>
-      </c>
-      <c r="I32" s="42">
-        <v>1.3320000000000001</v>
+        <v>5</v>
+      </c>
+      <c r="I32" s="8">
+        <f>IF(H32&lt;10,0.16,IF(H32&lt;25,0.111,0))</f>
+        <v>0.16</v>
       </c>
       <c r="J32" s="7">
-        <f>I32*H32</f>
-        <v>13.32</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="36" t="s">
-        <v>42</v>
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" s="73" t="s">
+        <v>130</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>43</v>
+        <v>131</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>7</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2">
-        <v>2</v>
-      </c>
-      <c r="I33" s="43">
-        <v>1.34</v>
+        <v>1</v>
+      </c>
+      <c r="I33" s="8">
+        <f>IF(H33&lt;10,0.14,IF(H33&lt;50,0.105))</f>
+        <v>0.14000000000000001</v>
       </c>
       <c r="J33" s="7">
-        <f t="shared" ref="J33:J34" si="0">I33*H33</f>
-        <v>2.68</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="36" t="s">
-        <v>33</v>
+        <f t="shared" si="1"/>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B34" s="73" t="s">
+        <v>134</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>25</v>
+        <v>124</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>136</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F34" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>7</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2">
         <v>1</v>
       </c>
-      <c r="I34" s="43">
-        <v>0.73</v>
+      <c r="I34" s="8">
+        <f>IF(H34&lt;10,0.15,IF(H34&lt;100,0.055,IF(H34&lt;1000,0.0222)))</f>
+        <v>0.15</v>
       </c>
       <c r="J34" s="7">
-        <f t="shared" si="0"/>
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="36" t="s">
-        <v>37</v>
+        <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B35" s="73" t="s">
+        <v>138</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>34</v>
+        <v>124</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>137</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F35" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>7</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2">
         <v>1</v>
       </c>
-      <c r="I35" s="43">
+      <c r="I35" s="8">
+        <f>IF(H35&lt;10,0.15,IF(H35&lt;100,0.058,IF(H35&lt;1000,0.0239)))</f>
+        <v>0.15</v>
+      </c>
+      <c r="J35" s="7">
+        <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B36" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2">
+        <v>1</v>
+      </c>
+      <c r="I36" s="8">
+        <v>2.67</v>
+      </c>
+      <c r="J36" s="7">
+        <f t="shared" si="1"/>
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B37" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2">
+        <v>1</v>
+      </c>
+      <c r="I37" s="8">
         <v>1.58</v>
       </c>
-      <c r="J35" s="7">
-        <f>I35*H35</f>
+      <c r="J37" s="7">
+        <f>I37*H37</f>
         <v>1.58</v>
       </c>
     </row>
-    <row r="36" spans="2:10" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="37" t="s">
+    <row r="38" spans="2:10" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B38" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C38" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D38" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11">
+        <v>1</v>
+      </c>
+      <c r="I38" s="17">
+        <v>1.55</v>
+      </c>
+      <c r="J38" s="18">
+        <f>I38*H38</f>
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B39" s="88" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="89"/>
+      <c r="D39" s="89"/>
+      <c r="E39" s="89"/>
+      <c r="F39" s="89"/>
+      <c r="G39" s="89"/>
+      <c r="H39" s="89"/>
+      <c r="I39" s="89"/>
+      <c r="J39" s="18">
+        <f>SUM(J29:J38)</f>
+        <v>22.080000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="9"/>
+    </row>
+    <row r="41" spans="2:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="9"/>
+    </row>
+    <row r="42" spans="2:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="43" spans="2:10" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B43" s="90" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" s="91"/>
+      <c r="D43" s="91"/>
+      <c r="E43" s="91"/>
+      <c r="F43" s="91"/>
+      <c r="G43" s="91"/>
+      <c r="H43" s="91"/>
+      <c r="I43" s="91"/>
+      <c r="J43" s="92"/>
+    </row>
+    <row r="44" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B44" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="I44" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J44" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B45" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F36" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11">
-        <v>1</v>
-      </c>
-      <c r="I36" s="44">
-        <v>1.58</v>
-      </c>
-      <c r="J36" s="18">
-        <f>I36*H36</f>
-        <v>1.58</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="91" t="s">
-        <v>28</v>
-      </c>
-      <c r="C37" s="92"/>
-      <c r="D37" s="92"/>
-      <c r="E37" s="92"/>
-      <c r="F37" s="92"/>
-      <c r="G37" s="92"/>
-      <c r="H37" s="92"/>
-      <c r="I37" s="92"/>
-      <c r="J37" s="18">
-        <f>SUM(J32:J36)</f>
-        <v>19.89</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="9"/>
-    </row>
-    <row r="39" spans="2:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="9"/>
-    </row>
-    <row r="40" spans="2:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="2:10" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="93" t="s">
-        <v>41</v>
-      </c>
-      <c r="C41" s="94"/>
-      <c r="D41" s="94"/>
-      <c r="E41" s="94"/>
-      <c r="F41" s="94"/>
-      <c r="G41" s="94"/>
-      <c r="H41" s="94"/>
-      <c r="I41" s="94"/>
-      <c r="J41" s="95"/>
-    </row>
-    <row r="42" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F42" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="I42" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="J42" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="C43" s="2" t="s">
+      <c r="C45" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="F45" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2">
-        <v>1</v>
-      </c>
-      <c r="I43" s="8">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="J43" s="7">
-        <f>I43*H43</f>
-        <v>2.3199999999999998</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D44" s="70" t="s">
-        <v>93</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2">
-        <v>1</v>
-      </c>
-      <c r="I44" s="8">
-        <v>54.48</v>
-      </c>
-      <c r="J44" s="39">
-        <f t="shared" ref="J44:J48" si="1">I44*H44</f>
-        <v>54.48</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D45" s="2">
-        <v>8341</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2">
         <v>1</v>
       </c>
       <c r="I45" s="8">
-        <v>15</v>
-      </c>
-      <c r="J45" s="39">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="J45" s="7">
+        <f>I45*H45</f>
+        <v>2.3199999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B46" s="36" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>92</v>
+        <v>47</v>
+      </c>
+      <c r="D46" s="69" t="s">
+        <v>89</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2">
         <v>1</v>
       </c>
       <c r="I46" s="8">
-        <v>10</v>
+        <v>54.48</v>
       </c>
       <c r="J46" s="39">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" ref="J46:J50" si="2">I46*H46</f>
+        <v>54.48</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B47" s="36" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>26</v>
+        <v>84</v>
+      </c>
+      <c r="D47" s="2">
+        <v>8341</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>26</v>
@@ -2590,78 +2606,114 @@
         <v>1</v>
       </c>
       <c r="I47" s="8">
+        <v>15</v>
+      </c>
+      <c r="J47" s="39">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B48" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2">
+        <v>1</v>
+      </c>
+      <c r="I48" s="8">
+        <v>10</v>
+      </c>
+      <c r="J48" s="39">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B49" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2">
+        <v>1</v>
+      </c>
+      <c r="I49" s="8">
         <v>5</v>
       </c>
-      <c r="J47" s="39">
-        <f t="shared" si="1"/>
+      <c r="J49" s="39">
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="2:10" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="C48" s="11" t="s">
+    <row r="50" spans="2:10" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B50" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D48" s="11" t="s">
+      <c r="D50" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="11" t="s">
+      <c r="E50" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F48" s="11" t="s">
+      <c r="F50" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11">
+      <c r="G50" s="11"/>
+      <c r="H50" s="11">
         <v>1</v>
       </c>
-      <c r="I48" s="17">
+      <c r="I50" s="17">
         <v>13</v>
       </c>
-      <c r="J48" s="18">
-        <f t="shared" si="1"/>
+      <c r="J50" s="18">
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="2:10" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="91" t="s">
+    <row r="51" spans="2:10" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B51" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="C49" s="92"/>
-      <c r="D49" s="92"/>
-      <c r="E49" s="92"/>
-      <c r="F49" s="92"/>
-      <c r="G49" s="92"/>
-      <c r="H49" s="92"/>
-      <c r="I49" s="92"/>
-      <c r="J49" s="18">
-        <f>SUM(J43:J48)</f>
+      <c r="C51" s="89"/>
+      <c r="D51" s="89"/>
+      <c r="E51" s="89"/>
+      <c r="F51" s="89"/>
+      <c r="G51" s="89"/>
+      <c r="H51" s="89"/>
+      <c r="I51" s="89"/>
+      <c r="J51" s="18">
+        <f>SUM(J45:J50)</f>
         <v>99.8</v>
       </c>
     </row>
-    <row r="50" spans="2:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="8"/>
-      <c r="J50" s="9"/>
-    </row>
-    <row r="51" spans="2:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="8"/>
-      <c r="J51" s="9"/>
-    </row>
-    <row r="52" spans="2:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -2671,338 +2723,379 @@
       <c r="I52" s="8"/>
       <c r="J52" s="9"/>
     </row>
-    <row r="53" spans="2:10" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="93" t="s">
-        <v>79</v>
-      </c>
-      <c r="C53" s="94"/>
-      <c r="D53" s="94"/>
-      <c r="E53" s="94"/>
-      <c r="F53" s="94"/>
-      <c r="G53" s="94"/>
-      <c r="H53" s="94"/>
-      <c r="I53" s="94"/>
-      <c r="J53" s="95"/>
-    </row>
-    <row r="54" spans="2:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="19" t="s">
+    <row r="53" spans="2:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="9"/>
+    </row>
+    <row r="54" spans="2:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="9"/>
+    </row>
+    <row r="55" spans="2:10" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B55" s="90" t="s">
+        <v>75</v>
+      </c>
+      <c r="C55" s="91"/>
+      <c r="D55" s="91"/>
+      <c r="E55" s="91"/>
+      <c r="F55" s="91"/>
+      <c r="G55" s="91"/>
+      <c r="H55" s="91"/>
+      <c r="I55" s="91"/>
+      <c r="J55" s="92"/>
+    </row>
+    <row r="56" spans="2:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B56" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C54" s="13" t="s">
+      <c r="C56" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D54" s="12" t="s">
+      <c r="D56" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="13" t="s">
+      <c r="E56" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F54" s="13" t="s">
+      <c r="F56" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14" t="s">
+      <c r="G56" s="14"/>
+      <c r="H56" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="I54" s="14" t="s">
+      <c r="I56" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="J54" s="33" t="s">
+      <c r="J56" s="33" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="40" t="s">
-        <v>102</v>
-      </c>
-      <c r="C55" s="35" t="s">
+    <row r="57" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B57" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C57" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="D57" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="E57" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="D55" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="E55" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="F55" s="35" t="s">
+      <c r="F57" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="G55" s="35"/>
-      <c r="H55" s="35">
+      <c r="G57" s="35"/>
+      <c r="H57" s="35">
         <v>10</v>
       </c>
-      <c r="I55" s="41">
+      <c r="I57" s="41">
+        <f>IF(H57&lt;10,0.69,IF(H57&lt;25,0.478,0))</f>
         <v>0.47799999999999998</v>
       </c>
-      <c r="J55" s="52">
-        <f>I55*H55</f>
+      <c r="J57" s="51">
+        <f>I57*H57</f>
         <v>4.7799999999999994</v>
       </c>
     </row>
-    <row r="56" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="36" t="s">
-        <v>94</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2">
-        <v>2</v>
-      </c>
-      <c r="I56" s="8">
-        <v>1.47</v>
-      </c>
-      <c r="J56" s="7">
-        <f t="shared" ref="J56:J60" si="2">I56*H56</f>
-        <v>2.94</v>
-      </c>
-    </row>
-    <row r="57" spans="2:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="71" t="s">
-        <v>98</v>
-      </c>
-      <c r="C57" s="73" t="s">
-        <v>99</v>
-      </c>
-      <c r="D57" s="72" t="s">
-        <v>100</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G57" s="2"/>
-      <c r="H57" s="2">
-        <v>10</v>
-      </c>
-      <c r="I57" s="8">
-        <v>0.49</v>
-      </c>
-      <c r="J57" s="7">
-        <f t="shared" si="2"/>
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="58" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="75" t="s">
-        <v>103</v>
+    <row r="58" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B58" s="36" t="s">
+        <v>90</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="G58" s="2"/>
       <c r="H58" s="2">
+        <v>2</v>
+      </c>
+      <c r="I58" s="8">
+        <v>1.47</v>
+      </c>
+      <c r="J58" s="7">
+        <f t="shared" ref="J58:J62" si="3">I58*H58</f>
+        <v>2.94</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B59" s="70" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59" s="76" t="s">
+        <v>95</v>
+      </c>
+      <c r="D59" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2">
+        <v>10</v>
+      </c>
+      <c r="I59" s="8">
+        <v>0.49</v>
+      </c>
+      <c r="J59" s="7">
+        <f t="shared" si="3"/>
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B60" s="73" t="s">
+        <v>99</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2">
         <v>20</v>
       </c>
-      <c r="I58" s="76">
+      <c r="I60" s="43">
+        <f>IF(H60&lt;10,0.14,IF(H60&lt;50,0.105,IF(H60&lt;100,0.0576,0)))</f>
         <v>0.105</v>
       </c>
-      <c r="J58" s="7">
-        <f t="shared" si="2"/>
+      <c r="J60" s="7">
+        <f t="shared" si="3"/>
         <v>2.1</v>
       </c>
     </row>
-    <row r="59" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="4"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
-      <c r="J59" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="2:10" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="10"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
-      <c r="G60" s="11"/>
-      <c r="H60" s="11"/>
-      <c r="I60" s="11"/>
-      <c r="J60" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="2:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="83" t="s">
+    <row r="61" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B61" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2">
+        <v>2</v>
+      </c>
+      <c r="I61" s="8">
+        <v>0.35</v>
+      </c>
+      <c r="J61" s="7">
+        <f t="shared" si="3"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B62" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E62" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="F62" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11">
+        <v>2</v>
+      </c>
+      <c r="I62" s="17">
+        <f>IF(H62&lt;10,0.28,IF(H62&lt;100,0.256,0))</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="J62" s="18">
+        <f t="shared" si="3"/>
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B63" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="C61" s="84"/>
-      <c r="D61" s="84"/>
-      <c r="E61" s="84"/>
-      <c r="F61" s="84"/>
-      <c r="G61" s="84"/>
-      <c r="H61" s="84"/>
-      <c r="I61" s="84"/>
-      <c r="J61" s="18">
-        <f>SUM(J55:J60)</f>
-        <v>14.719999999999999</v>
-      </c>
-    </row>
-    <row r="63" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="2:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="93" t="s">
-        <v>56</v>
-      </c>
-      <c r="C64" s="94"/>
-      <c r="D64" s="94"/>
-      <c r="E64" s="94"/>
-      <c r="F64" s="94"/>
-      <c r="G64" s="95"/>
-    </row>
-    <row r="65" spans="2:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="48" t="s">
+      <c r="C63" s="83"/>
+      <c r="D63" s="83"/>
+      <c r="E63" s="83"/>
+      <c r="F63" s="83"/>
+      <c r="G63" s="83"/>
+      <c r="H63" s="83"/>
+      <c r="I63" s="83"/>
+      <c r="J63" s="18">
+        <f>SUM(J57:J62)</f>
+        <v>15.979999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="66" spans="2:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B66" s="90" t="s">
+        <v>54</v>
+      </c>
+      <c r="C66" s="91"/>
+      <c r="D66" s="91"/>
+      <c r="E66" s="91"/>
+      <c r="F66" s="91"/>
+      <c r="G66" s="92"/>
+    </row>
+    <row r="67" spans="2:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B67" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C65" s="49" t="s">
+      <c r="C67" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="D67" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="E67" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="F67" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="G67" s="33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B68" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C68" s="71" t="s">
+        <v>114</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D65" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="E65" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="F65" s="49" t="s">
+      <c r="E68" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="F68" s="53">
+        <v>5</v>
+      </c>
+      <c r="G68" s="54">
+        <f>1.35*F68</f>
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B69" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="G65" s="33" t="s">
+      <c r="C69" s="11">
+        <v>4</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E69" s="55" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="66" spans="2:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C66" s="72">
-        <v>4</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E66" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="F66" s="54">
+      <c r="F69" s="56">
         <v>25.97</v>
       </c>
-      <c r="G66" s="55">
-        <f>1.35*F66</f>
+      <c r="G69" s="57">
+        <f>1.35*F69</f>
         <v>35.0595</v>
       </c>
     </row>
-    <row r="67" spans="2:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="C67" s="11">
-        <v>4</v>
-      </c>
-      <c r="D67" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E67" s="56" t="s">
-        <v>71</v>
-      </c>
-      <c r="F67" s="57">
-        <v>25.97</v>
-      </c>
-      <c r="G67" s="58">
-        <f>1.35*F67</f>
-        <v>35.0595</v>
-      </c>
-    </row>
-    <row r="68" spans="2:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="91" t="s">
+    <row r="70" spans="2:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B70" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="C68" s="92"/>
-      <c r="D68" s="92"/>
-      <c r="E68" s="92"/>
-      <c r="F68" s="92"/>
-      <c r="G68" s="59">
-        <f>SUM(G66:G67)</f>
-        <v>70.119</v>
-      </c>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-    </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
+      <c r="C70" s="89"/>
+      <c r="D70" s="89"/>
+      <c r="E70" s="89"/>
+      <c r="F70" s="89"/>
+      <c r="G70" s="58">
+        <f>SUM(G68:G69)</f>
+        <v>41.8095</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="B18:J18"/>
-    <mergeCell ref="B30:J30"/>
-    <mergeCell ref="B37:I37"/>
-    <mergeCell ref="B26:I26"/>
+  <mergeCells count="26">
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="B8:G8"/>
     <mergeCell ref="B2:J2"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="B70:F70"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="L9:M9"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="B66:G66"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="B18:J18"/>
+    <mergeCell ref="B27:J27"/>
+    <mergeCell ref="B39:I39"/>
     <mergeCell ref="L14:M14"/>
-    <mergeCell ref="B61:I61"/>
-    <mergeCell ref="B49:I49"/>
-    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="B63:I63"/>
+    <mergeCell ref="B51:I51"/>
+    <mergeCell ref="B43:J43"/>
+    <mergeCell ref="B55:J55"/>
     <mergeCell ref="L19:M19"/>
-    <mergeCell ref="B41:J41"/>
-    <mergeCell ref="B53:J53"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="B23:I23"/>
   </mergeCells>
   <conditionalFormatting sqref="N6">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
@@ -3012,7 +3105,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N20:O24">
+  <conditionalFormatting sqref="N21:O22 N19:O19">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3020,7 +3113,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N16:O16">
+  <conditionalFormatting sqref="N15:O15">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3044,14 +3137,14 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
-    <col min="4" max="7" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.26171875" customWidth="1"/>
+    <col min="3" max="3" width="28.26171875" customWidth="1"/>
+    <col min="4" max="7" width="24.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -3063,7 +3156,7 @@
       <c r="J2" s="20"/>
       <c r="K2" s="20"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="19" t="s">
         <v>3</v>
       </c>
@@ -3087,7 +3180,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
@@ -3112,7 +3205,7 @@
       <c r="J4" s="6"/>
       <c r="K4" s="9"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
@@ -3126,7 +3219,7 @@
       <c r="J5" s="6"/>
       <c r="K5" s="9"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
@@ -3151,7 +3244,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="9"/>
     </row>
-    <row r="7" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B7" s="29" t="s">
         <v>28</v>
       </c>

</xml_diff>